<commit_message>
add result asset & update benchmark
</commit_message>
<xml_diff>
--- a/experiment_benchmark.xlsx
+++ b/experiment_benchmark.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ReydVires\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\PCD\Tubes\webgl-canvas-image-proc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Process Time (ms)</t>
   </si>
   <si>
-    <t>Memory (KB)</t>
-  </si>
-  <si>
     <t>Histogram</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>exp_3.png</t>
+  </si>
+  <si>
+    <t>Memory (MB)</t>
   </si>
 </sst>
 </file>
@@ -223,22 +223,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -266,7 +285,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,386 +623,434 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16">
+        <v>4139606</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="25">
+        <f>AVERAGE(H5:H7)</f>
+        <v>2092.320000015508</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7">
+        <v>382.36500002676598</v>
+      </c>
+      <c r="I5" s="11">
+        <v>45.7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8">
+        <v>911.80500003974805</v>
+      </c>
+      <c r="I6" s="12">
+        <v>45.7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7">
+        <v>4982.7899999800102</v>
+      </c>
+      <c r="I7" s="11">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" ref="F8" si="0">AVERAGE(H8:H10)</f>
+        <v>143</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>99</v>
+      </c>
+      <c r="I8" s="13">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="10">
+        <v>254</v>
+      </c>
+      <c r="I9" s="14">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="9">
+        <v>76</v>
+      </c>
+      <c r="I10" s="13">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>2</v>
+      </c>
+      <c r="C11" s="19">
+        <v>150418</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="E11" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" ref="F11" si="1">AVERAGE(H11:H13)</f>
+        <v>84.006666690887229</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>16.7399999918416</v>
+      </c>
+      <c r="I11" s="7">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="8">
+        <v>43.480000051204101</v>
+      </c>
+      <c r="I12" s="8">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="7">
+        <v>191.800000029616</v>
+      </c>
+      <c r="I13" s="7">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25">
+        <f t="shared" ref="F14" si="2">AVERAGE(H14:H16)</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+      <c r="I14" s="13">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="10">
+        <v>14</v>
+      </c>
+      <c r="I15" s="14">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C17" s="22">
+        <v>187330</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" ref="F17" si="3">AVERAGE(H17:H19)</f>
+        <v>62.28833333201073</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="7">
+        <v>15.260000014677599</v>
+      </c>
+      <c r="I17" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="8">
+        <v>15.2949999901466</v>
+      </c>
+      <c r="I18" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="7">
+        <v>156.309999991208</v>
+      </c>
+      <c r="I19" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="F20" s="25">
+        <f t="shared" ref="F20" si="4">AVERAGE(H20:H22)</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>2</v>
+      </c>
+      <c r="I20" s="13">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>4139606</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.20083300000000001</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>386.11500000000001</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="H21" s="10">
+        <v>11</v>
+      </c>
+      <c r="I21" s="14">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="5">
-        <v>931.66499999999996</v>
-      </c>
-      <c r="I6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="4">
-        <v>5295.8249999999998</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12">
-        <v>150418</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.223333</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4">
-        <v>17.4800000386312</v>
-      </c>
-      <c r="I11" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5">
-        <v>43.480000051204101</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4">
-        <v>199.28500003879799</v>
-      </c>
-      <c r="I13" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
-        <v>3</v>
-      </c>
-      <c r="C17" s="15">
-        <v>187330</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.215</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>15.260000014677599</v>
-      </c>
-      <c r="I17" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5">
-        <v>15.2949999901466</v>
-      </c>
-      <c r="I18" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="4">
-        <v>156.309999991208</v>
-      </c>
-      <c r="I19" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="13">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E8:E10"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E8:E10"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="F8:F10"/>
@@ -984,10 +1059,13 @@
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="F20:F22"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="B2:I3"/>
-    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
* koreksi file excel
</commit_message>
<xml_diff>
--- a/experiment_benchmark.xlsx
+++ b/experiment_benchmark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15350" windowHeight="5870"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="15350" windowHeight="5870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Process Time (ms)</t>
   </si>
   <si>
-    <t>Memory (KB)</t>
-  </si>
-  <si>
     <t>Histogram</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>2.63 MB</t>
+  </si>
+  <si>
+    <t>Memory (MB)</t>
   </si>
 </sst>
 </file>
@@ -285,10 +285,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +577,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,7 +594,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -628,7 +628,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
@@ -650,11 +650,12 @@
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17">
-        <v>0.20083300000000001</v>
+      <c r="F5" s="16">
+        <f>AVERAGE(H5:H7)</f>
+        <v>2204.5349999999999</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>2</v>
@@ -670,10 +671,10 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="3">
         <v>931.66499999999996</v>
@@ -686,10 +687,10 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
         <v>5295.8249999999998</v>
@@ -702,10 +703,10 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="16">
+      <c r="E8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="17">
         <f>AVERAGE(H8:H10)</f>
         <v>143</v>
       </c>
@@ -716,39 +717,39 @@
         <v>99</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="4">
         <v>254</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="5">
         <v>76</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
@@ -759,13 +760,14 @@
         <v>150418</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="17">
-        <v>0.223333</v>
+      <c r="F11" s="16">
+        <f>AVERAGE(H11:H13)</f>
+        <v>86.748333376211107</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2</v>
@@ -781,10 +783,10 @@
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" s="3">
         <v>43.480000051204101</v>
@@ -797,10 +799,10 @@
       <c r="B13" s="8"/>
       <c r="C13" s="11"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2">
         <v>199.28500003879799</v>
@@ -813,10 +815,10 @@
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="16">
+      <c r="E14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="17">
         <f>AVERAGE(H14:H16)</f>
         <v>5.333333333333333</v>
       </c>
@@ -827,39 +829,39 @@
         <v>1</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4">
         <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="9"/>
       <c r="C16" s="12"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
@@ -870,13 +872,14 @@
         <v>187330</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="17">
-        <v>0.215</v>
+      <c r="F17" s="16">
+        <f>AVERAGE(H17:H19)</f>
+        <v>62.28833333201073</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>2</v>
@@ -892,10 +895,10 @@
       <c r="B18" s="8"/>
       <c r="C18" s="14"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="3">
         <v>15.2949999901466</v>
@@ -908,10 +911,10 @@
       <c r="B19" s="8"/>
       <c r="C19" s="14"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2">
         <v>156.309999991208</v>
@@ -924,10 +927,10 @@
       <c r="B20" s="8"/>
       <c r="C20" s="14"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="16">
+      <c r="E20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="17">
         <f>AVERAGE(H20:H22)</f>
         <v>5.333333333333333</v>
       </c>
@@ -938,68 +941,68 @@
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="8"/>
       <c r="C21" s="14"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H21" s="4">
         <v>11</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="9"/>
       <c r="C22" s="15"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" s="5">
         <v>3</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
         <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1009,6 +1012,8 @@
     <mergeCell ref="B2:I3"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B16"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="F8:F10"/>
@@ -1017,8 +1022,6 @@
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="F20:F22"/>
     <mergeCell ref="E14:E16"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="D5:D10"/>

</xml_diff>